<commit_message>
add spreadsheet for salt marsh protocol
</commit_message>
<xml_diff>
--- a/saltmarsh/original_fieldsheets/marinegeo_marsh_allometry_datasheet.xlsx
+++ b/saltmarsh/original_fieldsheets/marinegeo_marsh_allometry_datasheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CollabProj\MarineGEO SERC\Marsh Plant Surveys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\saltmarsh\original_fieldsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB05B5F-7732-4D14-8076-AADD67B160EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ECA152-94FD-4601-9598-8B4830272A3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="840" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Quad</t>
   </si>
@@ -102,74 +102,13 @@
     <t>Transect #</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Latitude of transect beginning </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Longitude of transect beginning </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Latitidue of transect ending  </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Longitude of transect ending</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 2</t>
-    </r>
-  </si>
-  <si>
     <t>Personnel</t>
   </si>
   <si>
     <t>Date (YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>Salt Marsh Plant Allometry</t>
   </si>
   <si>
     <r>
@@ -193,30 +132,6 @@
       </rPr>
       <t xml:space="preserve"> MarineGEO Site Codes can be found at marinegeo.github.io/standards; </t>
     </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> In Decimal Degrees to 5 decimal places (e.g. -43.12345, 142.12345)</t>
-    </r>
-  </si>
-  <si>
-    <t>Salt Marsh Plant Allometry</t>
   </si>
 </sst>
 </file>
@@ -277,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -672,68 +587,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -767,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -790,33 +643,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -830,58 +656,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -901,6 +675,72 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1182,10 +1022,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD40"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AD38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="AF5" sqref="AF5"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="96" zoomScaleNormal="120" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,351 +1065,347 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
+      <c r="A1" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
     </row>
     <row r="2" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="41" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="47" t="s">
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="36"/>
-    </row>
-    <row r="3" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="41" t="s">
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
-      <c r="AB3" s="39"/>
-    </row>
-    <row r="4" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="44" t="s">
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="33"/>
+    </row>
+    <row r="3" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="32"/>
-      <c r="X4" s="40"/>
-      <c r="Y4" s="40"/>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-    </row>
-    <row r="5" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="53"/>
-      <c r="Q5" s="53"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="53"/>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
-      <c r="V5" s="53"/>
-      <c r="W5" s="54"/>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="53"/>
-      <c r="AC5" s="53"/>
-      <c r="AD5" s="53"/>
-    </row>
-    <row r="6" spans="1:30" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="26"/>
+      <c r="AC3" s="26"/>
+      <c r="AD3" s="26"/>
+    </row>
+    <row r="4" spans="1:30" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B5" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D5" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14" t="s">
+      <c r="F5" s="44"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="14" t="s">
+      <c r="I5" s="44"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="14" t="s">
+      <c r="L5" s="44"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="14"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="14" t="s">
+      <c r="O5" s="44"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="14"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="14" t="s">
+      <c r="R5" s="44"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="U7" s="14"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="14" t="s">
+      <c r="U5" s="44"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="14" t="s">
+      <c r="X5" s="44"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="AA7" s="14"/>
+      <c r="AA5" s="44"/>
+      <c r="AB5" s="46"/>
+      <c r="AC5"/>
+    </row>
+    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="V6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="W6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC6"/>
+    </row>
+    <row r="7" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="2"/>
       <c r="AB7" s="16"/>
       <c r="AC7"/>
     </row>
-    <row r="8" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="S8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="T8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="V8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="W8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="X8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB8" s="12" t="s">
-        <v>7</v>
-      </c>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="17"/>
       <c r="AC8"/>
     </row>
-    <row r="9" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="25"/>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="17"/>
       <c r="AC9"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="1"/>
       <c r="C10" s="9"/>
       <c r="D10" s="6"/>
@@ -1593,11 +1432,11 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="26"/>
+      <c r="AB10" s="17"/>
       <c r="AC10"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="1"/>
       <c r="C11" s="9"/>
       <c r="D11" s="6"/>
@@ -1624,11 +1463,11 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="1"/>
-      <c r="AB11" s="26"/>
+      <c r="AB11" s="17"/>
       <c r="AC11"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="1"/>
       <c r="C12" s="9"/>
       <c r="D12" s="6"/>
@@ -1655,11 +1494,11 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="26"/>
+      <c r="AB12" s="17"/>
       <c r="AC12"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="1"/>
       <c r="C13" s="9"/>
       <c r="D13" s="6"/>
@@ -1686,11 +1525,11 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="1"/>
-      <c r="AB13" s="26"/>
+      <c r="AB13" s="17"/>
       <c r="AC13"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="1"/>
       <c r="C14" s="9"/>
       <c r="D14" s="6"/>
@@ -1717,11 +1556,11 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="1"/>
-      <c r="AB14" s="26"/>
+      <c r="AB14" s="17"/>
       <c r="AC14"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="1"/>
       <c r="C15" s="9"/>
       <c r="D15" s="6"/>
@@ -1748,11 +1587,11 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="7"/>
       <c r="AA15" s="1"/>
-      <c r="AB15" s="26"/>
+      <c r="AB15" s="17"/>
       <c r="AC15"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="1"/>
       <c r="C16" s="9"/>
       <c r="D16" s="6"/>
@@ -1779,11 +1618,11 @@
       <c r="Y16" s="6"/>
       <c r="Z16" s="7"/>
       <c r="AA16" s="1"/>
-      <c r="AB16" s="26"/>
+      <c r="AB16" s="17"/>
       <c r="AC16"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="1"/>
       <c r="C17" s="9"/>
       <c r="D17" s="6"/>
@@ -1810,11 +1649,11 @@
       <c r="Y17" s="6"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="26"/>
+      <c r="AB17" s="17"/>
       <c r="AC17"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="1"/>
       <c r="C18" s="9"/>
       <c r="D18" s="6"/>
@@ -1841,11 +1680,11 @@
       <c r="Y18" s="6"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="1"/>
-      <c r="AB18" s="26"/>
+      <c r="AB18" s="17"/>
       <c r="AC18"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="1"/>
       <c r="C19" s="9"/>
       <c r="D19" s="6"/>
@@ -1872,11 +1711,11 @@
       <c r="Y19" s="6"/>
       <c r="Z19" s="7"/>
       <c r="AA19" s="1"/>
-      <c r="AB19" s="26"/>
+      <c r="AB19" s="17"/>
       <c r="AC19"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="1"/>
       <c r="C20" s="9"/>
       <c r="D20" s="6"/>
@@ -1903,11 +1742,11 @@
       <c r="Y20" s="6"/>
       <c r="Z20" s="7"/>
       <c r="AA20" s="1"/>
-      <c r="AB20" s="26"/>
+      <c r="AB20" s="17"/>
       <c r="AC20"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="1"/>
       <c r="C21" s="9"/>
       <c r="D21" s="6"/>
@@ -1934,11 +1773,11 @@
       <c r="Y21" s="6"/>
       <c r="Z21" s="7"/>
       <c r="AA21" s="1"/>
-      <c r="AB21" s="26"/>
+      <c r="AB21" s="17"/>
       <c r="AC21"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="1"/>
       <c r="C22" s="9"/>
       <c r="D22" s="6"/>
@@ -1965,11 +1804,11 @@
       <c r="Y22" s="6"/>
       <c r="Z22" s="7"/>
       <c r="AA22" s="1"/>
-      <c r="AB22" s="26"/>
+      <c r="AB22" s="17"/>
       <c r="AC22"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="1"/>
       <c r="C23" s="9"/>
       <c r="D23" s="6"/>
@@ -1996,11 +1835,11 @@
       <c r="Y23" s="6"/>
       <c r="Z23" s="7"/>
       <c r="AA23" s="1"/>
-      <c r="AB23" s="26"/>
+      <c r="AB23" s="17"/>
       <c r="AC23"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="1"/>
       <c r="C24" s="9"/>
       <c r="D24" s="6"/>
@@ -2027,11 +1866,11 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="7"/>
       <c r="AA24" s="1"/>
-      <c r="AB24" s="26"/>
+      <c r="AB24" s="17"/>
       <c r="AC24"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="1"/>
       <c r="C25" s="9"/>
       <c r="D25" s="6"/>
@@ -2058,11 +1897,11 @@
       <c r="Y25" s="6"/>
       <c r="Z25" s="7"/>
       <c r="AA25" s="1"/>
-      <c r="AB25" s="26"/>
+      <c r="AB25" s="17"/>
       <c r="AC25"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="1"/>
       <c r="C26" s="9"/>
       <c r="D26" s="6"/>
@@ -2089,100 +1928,100 @@
       <c r="Y26" s="6"/>
       <c r="Z26" s="7"/>
       <c r="AA26" s="1"/>
-      <c r="AB26" s="26"/>
+      <c r="AB26" s="17"/>
       <c r="AC26"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="7"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="26"/>
+    <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="30"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="18"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="18"/>
+      <c r="Y27" s="20"/>
+      <c r="Z27" s="21"/>
+      <c r="AA27" s="18"/>
+      <c r="AB27" s="22"/>
       <c r="AC27"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="7"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="6"/>
-      <c r="Z28" s="7"/>
-      <c r="AA28" s="1"/>
-      <c r="AB28" s="26"/>
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
+      <c r="AB28"/>
       <c r="AC28"/>
     </row>
-    <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="57"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="29"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="29"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="29"/>
-      <c r="W29" s="30"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="29"/>
-      <c r="Z29" s="30"/>
-      <c r="AA29" s="27"/>
-      <c r="AB29" s="31"/>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+      <c r="Z29"/>
+      <c r="AA29"/>
+      <c r="AB29"/>
       <c r="AC29"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
@@ -2464,97 +2303,31 @@
       <c r="AB38"/>
       <c r="AC38"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-      <c r="N39"/>
-      <c r="O39"/>
-      <c r="P39"/>
-      <c r="Q39"/>
-      <c r="R39"/>
-      <c r="S39"/>
-      <c r="T39"/>
-      <c r="U39"/>
-      <c r="V39"/>
-      <c r="W39"/>
-      <c r="X39"/>
-      <c r="Y39"/>
-      <c r="Z39"/>
-      <c r="AA39"/>
-      <c r="AB39"/>
-      <c r="AC39"/>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-      <c r="O40"/>
-      <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-      <c r="S40"/>
-      <c r="T40"/>
-      <c r="U40"/>
-      <c r="V40"/>
-      <c r="W40"/>
-      <c r="X40"/>
-      <c r="Y40"/>
-      <c r="Z40"/>
-      <c r="AA40"/>
-      <c r="AB40"/>
-      <c r="AC40"/>
-    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="T2:AB3"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="K3:S3"/>
-    <mergeCell ref="K4:S4"/>
+  <mergeCells count="18">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="Z5:AB5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="T2:AB2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="O2:S2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="A1:AA1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="W7:Y7"/>
-    <mergeCell ref="Z7:AB7"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:V7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="1.0091145833333333" right="0.1" top="0.75" bottom="0.75" header="0.25" footer="0.25"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;CMarsh Plant Allometry</oddHeader>
+    <oddFooter>&amp;Lhttps://doi.org/10.25573/serc.14896194.v1</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>